<commit_message>
Re-organized TXL output files.
</commit_message>
<xml_diff>
--- a/doc/results.xlsx
+++ b/doc/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisa/Desktop/ConDesignPatterns/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5540E21-91ED-3849-B2B6-2424D7BCDB39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C37505-2318-AF44-826B-5596FDCAE16B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="460" windowWidth="27680" windowHeight="17540" xr2:uid="{A2A935D0-1E34-D741-B411-17C5D05EEFA3}"/>
   </bookViews>
@@ -1106,66 +1106,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1216,6 +1156,66 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1571,82 +1571,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="83" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="66" t="s">
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="66" t="s">
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="83" t="s">
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="66" t="s">
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="89"/>
+      <c r="AA1" s="89"/>
+      <c r="AB1" s="89"/>
+      <c r="AC1" s="89"/>
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="67"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="66" t="s">
+      <c r="AF1" s="84"/>
+      <c r="AG1" s="84"/>
+      <c r="AH1" s="84"/>
+      <c r="AI1" s="84"/>
+      <c r="AJ1" s="84"/>
+      <c r="AK1" s="84"/>
+      <c r="AL1" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="66" t="s">
+      <c r="AM1" s="84"/>
+      <c r="AN1" s="84"/>
+      <c r="AO1" s="84"/>
+      <c r="AP1" s="84"/>
+      <c r="AQ1" s="84"/>
+      <c r="AR1" s="85"/>
+      <c r="AS1" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="67"/>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="67"/>
-      <c r="AX1" s="67"/>
-      <c r="AY1" s="68"/>
-      <c r="AZ1" s="66" t="s">
+      <c r="AT1" s="84"/>
+      <c r="AU1" s="84"/>
+      <c r="AV1" s="84"/>
+      <c r="AW1" s="84"/>
+      <c r="AX1" s="84"/>
+      <c r="AY1" s="85"/>
+      <c r="AZ1" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" s="67"/>
-      <c r="BB1" s="67"/>
-      <c r="BC1" s="67"/>
-      <c r="BD1" s="67"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="68"/>
+      <c r="BA1" s="84"/>
+      <c r="BB1" s="84"/>
+      <c r="BC1" s="84"/>
+      <c r="BD1" s="84"/>
+      <c r="BE1" s="84"/>
+      <c r="BF1" s="85"/>
     </row>
     <row r="2" spans="1:58" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1655,25 +1655,25 @@
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="87" t="s">
+      <c r="D2" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="87" t="s">
+      <c r="E2" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="87" t="s">
+      <c r="F2" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="87" t="s">
+      <c r="G2" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="87" t="s">
+      <c r="H2" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="88" t="s">
+      <c r="I2" s="68" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="6" t="s">
@@ -1718,25 +1718,25 @@
       <c r="W2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="X2" s="86" t="s">
+      <c r="X2" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="87" t="s">
+      <c r="Y2" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" s="87" t="s">
+      <c r="Z2" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="AA2" s="87" t="s">
+      <c r="AA2" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="AB2" s="87" t="s">
+      <c r="AB2" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="87" t="s">
+      <c r="AC2" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="AD2" s="88" t="s">
+      <c r="AD2" s="68" t="s">
         <v>11</v>
       </c>
       <c r="AE2" s="6" t="s">
@@ -1831,27 +1831,27 @@
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="89">
+      <c r="C3" s="69">
         <v>37</v>
       </c>
-      <c r="D3" s="99">
+      <c r="D3" s="79">
         <v>36</v>
       </c>
-      <c r="E3" s="99">
-        <v>0</v>
-      </c>
-      <c r="F3" s="100">
+      <c r="E3" s="79">
+        <v>0</v>
+      </c>
+      <c r="F3" s="80">
         <f>D3/C3*100</f>
         <v>97.297297297297305</v>
       </c>
-      <c r="G3" s="100">
+      <c r="G3" s="80">
         <f>E3/C3*100</f>
         <v>0</v>
       </c>
-      <c r="H3" s="101" t="s">
-        <v>103</v>
-      </c>
-      <c r="I3" s="101" t="s">
+      <c r="H3" s="81" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="81" t="s">
         <v>103</v>
       </c>
       <c r="J3" s="14">
@@ -1896,25 +1896,25 @@
       <c r="W3" s="16">
         <v>0</v>
       </c>
-      <c r="X3" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB3" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC3" s="92">
+      <c r="X3" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB3" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC3" s="72">
         <v>3</v>
       </c>
-      <c r="AD3" s="90">
+      <c r="AD3" s="70">
         <v>0</v>
       </c>
       <c r="AE3" s="14">
@@ -2009,27 +2009,27 @@
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="89">
+      <c r="C4" s="69">
         <v>2</v>
       </c>
-      <c r="D4" s="90">
+      <c r="D4" s="70">
         <v>2</v>
       </c>
-      <c r="E4" s="90">
-        <v>0</v>
-      </c>
-      <c r="F4" s="100">
+      <c r="E4" s="70">
+        <v>0</v>
+      </c>
+      <c r="F4" s="80">
         <f t="shared" ref="F4:F19" si="0">D4/C4*100</f>
         <v>100</v>
       </c>
-      <c r="G4" s="100">
+      <c r="G4" s="80">
         <f t="shared" ref="G4:G19" si="1">E4/C4*100</f>
         <v>0</v>
       </c>
-      <c r="H4" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I4" s="90" t="s">
+      <c r="H4" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J4" s="14">
@@ -2076,25 +2076,25 @@
       <c r="W4" s="16">
         <v>0</v>
       </c>
-      <c r="X4" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB4" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC4" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="90">
+      <c r="X4" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB4" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC4" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="70">
         <v>0</v>
       </c>
       <c r="AE4" s="14">
@@ -2189,27 +2189,27 @@
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="89">
+      <c r="C5" s="69">
         <v>2</v>
       </c>
-      <c r="D5" s="90">
+      <c r="D5" s="70">
         <v>2</v>
       </c>
-      <c r="E5" s="90">
-        <v>0</v>
-      </c>
-      <c r="F5" s="100">
+      <c r="E5" s="70">
+        <v>0</v>
+      </c>
+      <c r="F5" s="80">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G5" s="100">
+      <c r="G5" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H5" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="90" t="s">
+      <c r="H5" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J5" s="14">
@@ -2256,25 +2256,25 @@
       <c r="W5" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="X5" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB5" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC5" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="90">
+      <c r="X5" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB5" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC5" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="70">
         <v>0</v>
       </c>
       <c r="AE5" s="14">
@@ -2369,27 +2369,27 @@
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="89">
+      <c r="C6" s="69">
         <v>2</v>
       </c>
-      <c r="D6" s="90">
+      <c r="D6" s="70">
         <v>2</v>
       </c>
-      <c r="E6" s="90">
-        <v>0</v>
-      </c>
-      <c r="F6" s="100">
+      <c r="E6" s="70">
+        <v>0</v>
+      </c>
+      <c r="F6" s="80">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G6" s="100">
+      <c r="G6" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H6" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="102" t="s">
+      <c r="H6" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="82" t="s">
         <v>103</v>
       </c>
       <c r="J6" s="14">
@@ -2436,25 +2436,25 @@
       <c r="W6" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="X6" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB6" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC6" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="90">
+      <c r="X6" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB6" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC6" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="70">
         <v>0</v>
       </c>
       <c r="AE6" s="14">
@@ -2549,25 +2549,25 @@
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="89">
-        <v>0</v>
-      </c>
-      <c r="D7" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="100" t="s">
-        <v>103</v>
-      </c>
-      <c r="G7" s="100" t="s">
-        <v>103</v>
-      </c>
-      <c r="H7" s="90">
-        <v>0</v>
-      </c>
-      <c r="I7" s="102">
+      <c r="C7" s="69">
+        <v>0</v>
+      </c>
+      <c r="D7" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="70">
+        <v>0</v>
+      </c>
+      <c r="I7" s="82">
         <v>0</v>
       </c>
       <c r="J7" s="14">
@@ -2612,25 +2612,25 @@
       <c r="W7" s="16">
         <v>0</v>
       </c>
-      <c r="X7" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB7" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC7" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="90">
+      <c r="X7" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB7" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC7" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="70">
         <v>0</v>
       </c>
       <c r="AE7" s="14">
@@ -2725,25 +2725,25 @@
       <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="89">
-        <v>0</v>
-      </c>
-      <c r="D8" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" s="100" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" s="100" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="90">
-        <v>0</v>
-      </c>
-      <c r="I8" s="102">
+      <c r="C8" s="69">
+        <v>0</v>
+      </c>
+      <c r="D8" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="70">
+        <v>0</v>
+      </c>
+      <c r="I8" s="82">
         <v>0</v>
       </c>
       <c r="J8" s="14">
@@ -2788,25 +2788,25 @@
       <c r="W8" s="16">
         <v>0</v>
       </c>
-      <c r="X8" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB8" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC8" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="90">
+      <c r="X8" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB8" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC8" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="70">
         <v>0</v>
       </c>
       <c r="AE8" s="14">
@@ -2901,27 +2901,27 @@
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="89">
+      <c r="C9" s="69">
         <v>2</v>
       </c>
-      <c r="D9" s="90">
+      <c r="D9" s="70">
         <v>2</v>
       </c>
-      <c r="E9" s="90">
-        <v>0</v>
-      </c>
-      <c r="F9" s="100">
+      <c r="E9" s="70">
+        <v>0</v>
+      </c>
+      <c r="F9" s="80">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G9" s="100">
+      <c r="G9" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H9" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I9" s="90" t="s">
+      <c r="H9" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J9" s="14">
@@ -2968,25 +2968,25 @@
       <c r="W9" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="X9" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB9" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC9" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="90">
+      <c r="X9" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB9" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC9" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="70">
         <v>0</v>
       </c>
       <c r="AE9" s="14">
@@ -3083,27 +3083,27 @@
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="89">
+      <c r="C10" s="69">
         <v>7</v>
       </c>
-      <c r="D10" s="90">
+      <c r="D10" s="70">
         <v>7</v>
       </c>
-      <c r="E10" s="90">
-        <v>0</v>
-      </c>
-      <c r="F10" s="100">
+      <c r="E10" s="70">
+        <v>0</v>
+      </c>
+      <c r="F10" s="80">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G10" s="100">
+      <c r="G10" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I10" s="90" t="s">
+      <c r="H10" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J10" s="14">
@@ -3150,25 +3150,25 @@
       <c r="W10" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="X10" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB10" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC10" s="92">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="90">
+      <c r="X10" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB10" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC10" s="72">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="70">
         <v>0</v>
       </c>
       <c r="AE10" s="14">
@@ -3263,27 +3263,27 @@
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="89">
+      <c r="C11" s="69">
         <v>8</v>
       </c>
-      <c r="D11" s="90">
+      <c r="D11" s="70">
         <v>8</v>
       </c>
-      <c r="E11" s="90">
-        <v>0</v>
-      </c>
-      <c r="F11" s="100">
+      <c r="E11" s="70">
+        <v>0</v>
+      </c>
+      <c r="F11" s="80">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G11" s="100">
+      <c r="G11" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I11" s="90" t="s">
+      <c r="H11" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J11" s="14">
@@ -3330,25 +3330,25 @@
       <c r="W11" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="X11" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB11" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC11" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="90">
+      <c r="X11" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB11" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC11" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="70">
         <v>0</v>
       </c>
       <c r="AE11" s="14">
@@ -3443,27 +3443,27 @@
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="89">
+      <c r="C12" s="69">
         <v>2</v>
       </c>
-      <c r="D12" s="90">
+      <c r="D12" s="70">
         <v>2</v>
       </c>
-      <c r="E12" s="90">
-        <v>0</v>
-      </c>
-      <c r="F12" s="100">
+      <c r="E12" s="70">
+        <v>0</v>
+      </c>
+      <c r="F12" s="80">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G12" s="100">
+      <c r="G12" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I12" s="90" t="s">
+      <c r="H12" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J12" s="14">
@@ -3510,25 +3510,25 @@
       <c r="W12" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="X12" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB12" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC12" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="90">
+      <c r="X12" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB12" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC12" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="70">
         <v>0</v>
       </c>
       <c r="AE12" s="14">
@@ -3623,25 +3623,25 @@
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="89">
-        <v>0</v>
-      </c>
-      <c r="D13" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="E13" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="100" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" s="100" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="90">
-        <v>0</v>
-      </c>
-      <c r="I13" s="102">
+      <c r="C13" s="69">
+        <v>0</v>
+      </c>
+      <c r="D13" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="70">
+        <v>0</v>
+      </c>
+      <c r="I13" s="82">
         <v>0</v>
       </c>
       <c r="J13" s="14">
@@ -3686,25 +3686,25 @@
       <c r="W13" s="16">
         <v>0</v>
       </c>
-      <c r="X13" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB13" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC13" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="90">
+      <c r="X13" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB13" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC13" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="70">
         <v>0</v>
       </c>
       <c r="AE13" s="14">
@@ -3799,27 +3799,27 @@
       <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="89">
+      <c r="C14" s="69">
         <v>3</v>
       </c>
-      <c r="D14" s="99">
+      <c r="D14" s="79">
         <v>2</v>
       </c>
-      <c r="E14" s="99">
-        <v>0</v>
-      </c>
-      <c r="F14" s="100">
+      <c r="E14" s="79">
+        <v>0</v>
+      </c>
+      <c r="F14" s="80">
         <f t="shared" si="0"/>
         <v>66.666666666666657</v>
       </c>
-      <c r="G14" s="100">
+      <c r="G14" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" s="90" t="s">
+      <c r="H14" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J14" s="14">
@@ -3864,25 +3864,25 @@
       <c r="W14" s="16">
         <v>0</v>
       </c>
-      <c r="X14" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB14" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC14" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="90">
+      <c r="X14" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB14" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC14" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="70">
         <v>0</v>
       </c>
       <c r="AE14" s="14">
@@ -3979,27 +3979,27 @@
       <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="89">
+      <c r="C15" s="69">
         <v>44</v>
       </c>
-      <c r="D15" s="99">
+      <c r="D15" s="79">
         <v>32</v>
       </c>
-      <c r="E15" s="99">
-        <v>0</v>
-      </c>
-      <c r="F15" s="100">
+      <c r="E15" s="79">
+        <v>0</v>
+      </c>
+      <c r="F15" s="80">
         <f t="shared" si="0"/>
         <v>72.727272727272734</v>
       </c>
-      <c r="G15" s="100">
+      <c r="G15" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I15" s="90" t="s">
+      <c r="H15" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J15" s="14">
@@ -4044,27 +4044,27 @@
       <c r="W15" s="16">
         <v>0</v>
       </c>
-      <c r="X15" s="89">
+      <c r="X15" s="69">
         <v>36</v>
       </c>
-      <c r="Y15" s="93">
-        <v>1</v>
-      </c>
-      <c r="Z15" s="93">
+      <c r="Y15" s="73">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="73">
         <v>35</v>
       </c>
-      <c r="AA15" s="94">
+      <c r="AA15" s="74">
         <f>Y15/X15*100</f>
         <v>2.7777777777777777</v>
       </c>
-      <c r="AB15" s="94">
+      <c r="AB15" s="74">
         <f>Z15/X15*100</f>
         <v>97.222222222222214</v>
       </c>
-      <c r="AC15" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="AD15" s="90" t="s">
+      <c r="AC15" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD15" s="70" t="s">
         <v>103</v>
       </c>
       <c r="AE15" s="14">
@@ -4159,27 +4159,27 @@
       <c r="B16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="89">
+      <c r="C16" s="69">
         <v>5</v>
       </c>
-      <c r="D16" s="90">
+      <c r="D16" s="70">
         <v>5</v>
       </c>
-      <c r="E16" s="90">
-        <v>0</v>
-      </c>
-      <c r="F16" s="100">
+      <c r="E16" s="70">
+        <v>0</v>
+      </c>
+      <c r="F16" s="80">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G16" s="100">
+      <c r="G16" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I16" s="90" t="s">
+      <c r="H16" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I16" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J16" s="14">
@@ -4226,25 +4226,25 @@
       <c r="W16" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="X16" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB16" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC16" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="90">
+      <c r="X16" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB16" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC16" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="70">
         <v>0</v>
       </c>
       <c r="AE16" s="14">
@@ -4341,27 +4341,27 @@
       <c r="B17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="89">
+      <c r="C17" s="69">
         <v>4</v>
       </c>
-      <c r="D17" s="90">
+      <c r="D17" s="70">
         <v>4</v>
       </c>
-      <c r="E17" s="90">
-        <v>0</v>
-      </c>
-      <c r="F17" s="100">
+      <c r="E17" s="70">
+        <v>0</v>
+      </c>
+      <c r="F17" s="80">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G17" s="100">
+      <c r="G17" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H17" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I17" s="90" t="s">
+      <c r="H17" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J17" s="14">
@@ -4406,25 +4406,25 @@
       <c r="W17" s="3">
         <v>0</v>
       </c>
-      <c r="X17" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB17" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC17" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="90">
+      <c r="X17" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB17" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC17" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="70">
         <v>0</v>
       </c>
       <c r="AE17" s="14">
@@ -4521,27 +4521,27 @@
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="89">
+      <c r="C18" s="69">
         <v>2</v>
       </c>
-      <c r="D18" s="90">
+      <c r="D18" s="70">
         <v>2</v>
       </c>
-      <c r="E18" s="90">
-        <v>0</v>
-      </c>
-      <c r="F18" s="100">
+      <c r="E18" s="70">
+        <v>0</v>
+      </c>
+      <c r="F18" s="80">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G18" s="100">
+      <c r="G18" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H18" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I18" s="90" t="s">
+      <c r="H18" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J18" s="14">
@@ -4586,25 +4586,25 @@
       <c r="W18" s="3">
         <v>0</v>
       </c>
-      <c r="X18" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB18" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC18" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="90">
+      <c r="X18" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB18" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC18" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="70">
         <v>0</v>
       </c>
       <c r="AE18" s="14">
@@ -4701,27 +4701,27 @@
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="89">
+      <c r="C19" s="69">
         <v>2</v>
       </c>
-      <c r="D19" s="90">
+      <c r="D19" s="70">
         <v>2</v>
       </c>
-      <c r="E19" s="90">
-        <v>0</v>
-      </c>
-      <c r="F19" s="100">
+      <c r="E19" s="70">
+        <v>0</v>
+      </c>
+      <c r="F19" s="80">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G19" s="100">
+      <c r="G19" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="I19" s="90" t="s">
+      <c r="H19" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="70" t="s">
         <v>103</v>
       </c>
       <c r="J19" s="14">
@@ -4766,25 +4766,25 @@
       <c r="W19" s="16">
         <v>0</v>
       </c>
-      <c r="X19" s="89">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="90">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="90">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB19" s="91" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC19" s="90">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="90">
+      <c r="X19" s="69">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="70">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="70">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB19" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC19" s="70">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="70">
         <v>0</v>
       </c>
       <c r="AE19" s="14">
@@ -4878,31 +4878,31 @@
       <c r="B20" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="95">
+      <c r="C20" s="75">
         <f>SUM(C3:C19)</f>
         <v>122</v>
       </c>
-      <c r="D20" s="96">
+      <c r="D20" s="76">
         <f>SUM(D3:D19)</f>
         <v>108</v>
       </c>
-      <c r="E20" s="96">
+      <c r="E20" s="76">
         <f>SUM(E3:E19)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="97">
+      <c r="F20" s="77">
         <f>D20/C20*100</f>
         <v>88.52459016393442</v>
       </c>
-      <c r="G20" s="96">
+      <c r="G20" s="76">
         <f>E20/C20</f>
         <v>0</v>
       </c>
-      <c r="H20" s="96">
+      <c r="H20" s="76">
         <f>SUM(H3:H19)</f>
         <v>0</v>
       </c>
-      <c r="I20" s="98">
+      <c r="I20" s="78">
         <f>SUM(I3:I19)</f>
         <v>0</v>
       </c>
@@ -4962,31 +4962,31 @@
         <f>SUM(W3:W19)</f>
         <v>0</v>
       </c>
-      <c r="X20" s="95">
+      <c r="X20" s="75">
         <f>SUM(X3:X19)</f>
         <v>36</v>
       </c>
-      <c r="Y20" s="96">
+      <c r="Y20" s="76">
         <f>SUM(Y3:Y19)</f>
         <v>1</v>
       </c>
-      <c r="Z20" s="96">
+      <c r="Z20" s="76">
         <f>SUM(Z3:Z19)</f>
         <v>35</v>
       </c>
-      <c r="AA20" s="96">
+      <c r="AA20" s="76">
         <f>Y20/X20*100</f>
         <v>2.7777777777777777</v>
       </c>
-      <c r="AB20" s="96">
+      <c r="AB20" s="76">
         <f>Z20/X20*100</f>
         <v>97.222222222222214</v>
       </c>
-      <c r="AC20" s="97">
+      <c r="AC20" s="77">
         <f>SUM(AC3:AC19)</f>
         <v>4</v>
       </c>
-      <c r="AD20" s="98">
+      <c r="AD20" s="78">
         <f>SUM(AD3:AD19)</f>
         <v>0</v>
       </c>
@@ -5676,7 +5676,7 @@
       </c>
     </row>
     <row r="23" spans="1:29" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="82" t="s">
+      <c r="A23" s="102" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="3">
@@ -5711,7 +5711,7 @@
       <c r="AC23" s="48"/>
     </row>
     <row r="24" spans="1:29" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="82"/>
+      <c r="A24" s="102"/>
       <c r="B24" s="3">
         <v>2</v>
       </c>
@@ -5771,17 +5771,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="74" t="s">
+      <c r="B1" s="92"/>
+      <c r="C1" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="73"/>
+      <c r="E1" s="92"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
@@ -5790,7 +5790,7 @@
       <c r="B2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="93"/>
       <c r="D2" s="23" t="s">
         <v>51</v>
       </c>
@@ -5799,13 +5799,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="75">
+      <c r="C3" s="94">
         <v>37</v>
       </c>
       <c r="D3" s="24">
@@ -5816,9 +5816,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="72"/>
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="94"/>
       <c r="D4" s="24">
         <v>2</v>
       </c>
@@ -5828,9 +5828,9 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="72"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="75"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="94"/>
       <c r="D5" s="24">
         <v>3</v>
       </c>
@@ -5840,9 +5840,9 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="72"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="75"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="94"/>
       <c r="D6" s="24">
         <v>4</v>
       </c>
@@ -5852,9 +5852,9 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="72"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="75"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="94"/>
       <c r="D7" s="24">
         <v>5</v>
       </c>
@@ -5864,9 +5864,9 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="72"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="75"/>
+      <c r="A8" s="91"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="94"/>
       <c r="D8" s="24">
         <v>6</v>
       </c>
@@ -5876,9 +5876,9 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="72"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="75"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="94"/>
       <c r="D9" s="24">
         <v>7</v>
       </c>
@@ -5888,9 +5888,9 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="72"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="75"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="94"/>
       <c r="D10" s="24">
         <v>8</v>
       </c>
@@ -5900,9 +5900,9 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="72"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="75"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="94"/>
       <c r="D11" s="24">
         <v>9</v>
       </c>
@@ -5912,9 +5912,9 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="72"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="75"/>
+      <c r="A12" s="91"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="94"/>
       <c r="D12" s="24">
         <v>10</v>
       </c>
@@ -5924,9 +5924,9 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="72"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="75"/>
+      <c r="A13" s="91"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="94"/>
       <c r="D13" s="24">
         <v>11</v>
       </c>
@@ -5936,9 +5936,9 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="75"/>
+      <c r="A14" s="91"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="94"/>
       <c r="D14" s="24">
         <v>12</v>
       </c>
@@ -5948,9 +5948,9 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="72"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="75"/>
+      <c r="A15" s="91"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="94"/>
       <c r="D15" s="24">
         <v>13</v>
       </c>
@@ -5960,9 +5960,9 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="72"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="75"/>
+      <c r="A16" s="91"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="94"/>
       <c r="D16" s="24">
         <v>14</v>
       </c>
@@ -5972,9 +5972,9 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="72"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="75"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="94"/>
       <c r="D17" s="24">
         <v>15</v>
       </c>
@@ -5984,9 +5984,9 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="72"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="75"/>
+      <c r="A18" s="91"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="94"/>
       <c r="D18" s="24">
         <v>16</v>
       </c>
@@ -5996,9 +5996,9 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="72"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="75"/>
+      <c r="A19" s="91"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="94"/>
       <c r="D19" s="24">
         <v>17</v>
       </c>
@@ -6008,9 +6008,9 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="72"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="75"/>
+      <c r="A20" s="91"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="94"/>
       <c r="D20" s="24">
         <v>18</v>
       </c>
@@ -6020,9 +6020,9 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="72"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="75"/>
+      <c r="A21" s="91"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="94"/>
       <c r="D21" s="24">
         <v>19</v>
       </c>
@@ -6032,9 +6032,9 @@
       <c r="G21" s="29"/>
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="72"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="75"/>
+      <c r="A22" s="91"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="94"/>
       <c r="D22" s="24">
         <v>20</v>
       </c>
@@ -6043,9 +6043,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="72"/>
-      <c r="B23" s="72"/>
-      <c r="C23" s="75"/>
+      <c r="A23" s="91"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="94"/>
       <c r="D23" s="24">
         <v>21</v>
       </c>
@@ -6054,9 +6054,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="72"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="75"/>
+      <c r="A24" s="91"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="94"/>
       <c r="D24" s="24">
         <v>22</v>
       </c>
@@ -6065,9 +6065,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="72"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="75"/>
+      <c r="A25" s="91"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="94"/>
       <c r="D25" s="24">
         <v>23</v>
       </c>
@@ -6076,9 +6076,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="72"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="75"/>
+      <c r="A26" s="91"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="94"/>
       <c r="D26" s="24">
         <v>24</v>
       </c>
@@ -6087,9 +6087,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="72"/>
-      <c r="B27" s="72"/>
-      <c r="C27" s="75"/>
+      <c r="A27" s="91"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="94"/>
       <c r="D27" s="24">
         <v>25</v>
       </c>
@@ -6098,9 +6098,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="72"/>
-      <c r="B28" s="72"/>
-      <c r="C28" s="75"/>
+      <c r="A28" s="91"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="94"/>
       <c r="D28" s="24">
         <v>26</v>
       </c>
@@ -6109,9 +6109,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="72"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="75"/>
+      <c r="A29" s="91"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="94"/>
       <c r="D29" s="24">
         <v>27</v>
       </c>
@@ -6120,9 +6120,9 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="72"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="75"/>
+      <c r="A30" s="91"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="94"/>
       <c r="D30" s="24">
         <v>28</v>
       </c>
@@ -6131,9 +6131,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="72"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="75"/>
+      <c r="A31" s="91"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="94"/>
       <c r="D31" s="24">
         <v>29</v>
       </c>
@@ -6142,9 +6142,9 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="72"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="75"/>
+      <c r="A32" s="91"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="94"/>
       <c r="D32" s="24">
         <v>30</v>
       </c>
@@ -6153,9 +6153,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="72"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="75"/>
+      <c r="A33" s="91"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="94"/>
       <c r="D33" s="24">
         <v>31</v>
       </c>
@@ -6164,9 +6164,9 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="72"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="75"/>
+      <c r="A34" s="91"/>
+      <c r="B34" s="91"/>
+      <c r="C34" s="94"/>
       <c r="D34" s="24">
         <v>32</v>
       </c>
@@ -6175,9 +6175,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="72"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="75"/>
+      <c r="A35" s="91"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="94"/>
       <c r="D35" s="24">
         <v>33</v>
       </c>
@@ -6186,9 +6186,9 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="72"/>
-      <c r="B36" s="72"/>
-      <c r="C36" s="75"/>
+      <c r="A36" s="91"/>
+      <c r="B36" s="91"/>
+      <c r="C36" s="94"/>
       <c r="D36" s="24">
         <v>34</v>
       </c>
@@ -6197,9 +6197,9 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="72"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="75"/>
+      <c r="A37" s="91"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="94"/>
       <c r="D37" s="24">
         <v>35</v>
       </c>
@@ -6208,9 +6208,9 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="72"/>
-      <c r="B38" s="72"/>
-      <c r="C38" s="75"/>
+      <c r="A38" s="91"/>
+      <c r="B38" s="91"/>
+      <c r="C38" s="94"/>
       <c r="D38" s="24">
         <v>36</v>
       </c>
@@ -6219,9 +6219,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="72"/>
-      <c r="B39" s="72"/>
-      <c r="C39" s="75"/>
+      <c r="A39" s="91"/>
+      <c r="B39" s="91"/>
+      <c r="C39" s="94"/>
       <c r="D39" s="24">
         <v>37</v>
       </c>
@@ -6230,13 +6230,13 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="72" t="s">
+      <c r="A40" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="72" t="s">
+      <c r="B40" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="71">
+      <c r="C40" s="95">
         <v>2</v>
       </c>
       <c r="D40" s="24">
@@ -6247,9 +6247,9 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="72"/>
-      <c r="B41" s="72"/>
-      <c r="C41" s="71"/>
+      <c r="A41" s="91"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="95"/>
       <c r="D41" s="24">
         <v>2</v>
       </c>
@@ -6258,13 +6258,13 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="72" t="s">
+      <c r="A42" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="B42" s="72" t="s">
+      <c r="B42" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="71">
+      <c r="C42" s="95">
         <v>2</v>
       </c>
       <c r="D42" s="24">
@@ -6275,9 +6275,9 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="72"/>
-      <c r="B43" s="72"/>
-      <c r="C43" s="71"/>
+      <c r="A43" s="91"/>
+      <c r="B43" s="91"/>
+      <c r="C43" s="95"/>
       <c r="D43" s="24">
         <v>2</v>
       </c>
@@ -6286,13 +6286,13 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="72" t="s">
+      <c r="A44" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="71">
+      <c r="C44" s="95">
         <v>2</v>
       </c>
       <c r="D44" s="24">
@@ -6303,9 +6303,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="72"/>
-      <c r="B45" s="72"/>
-      <c r="C45" s="71"/>
+      <c r="A45" s="91"/>
+      <c r="B45" s="91"/>
+      <c r="C45" s="95"/>
       <c r="D45" s="24">
         <v>2</v>
       </c>
@@ -6348,13 +6348,13 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="72" t="s">
+      <c r="A48" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="71">
+      <c r="B48" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="95">
         <v>2</v>
       </c>
       <c r="D48" s="24">
@@ -6365,9 +6365,9 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="72"/>
-      <c r="B49" s="72"/>
-      <c r="C49" s="71"/>
+      <c r="A49" s="91"/>
+      <c r="B49" s="91"/>
+      <c r="C49" s="95"/>
       <c r="D49" s="24">
         <v>2</v>
       </c>
@@ -6376,13 +6376,13 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="72" t="s">
+      <c r="A50" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="72" t="s">
+      <c r="B50" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="71">
+      <c r="C50" s="95">
         <v>7</v>
       </c>
       <c r="D50" s="24">
@@ -6393,9 +6393,9 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="72"/>
-      <c r="B51" s="72"/>
-      <c r="C51" s="71"/>
+      <c r="A51" s="91"/>
+      <c r="B51" s="91"/>
+      <c r="C51" s="95"/>
       <c r="D51" s="24">
         <v>2</v>
       </c>
@@ -6404,9 +6404,9 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="72"/>
-      <c r="B52" s="72"/>
-      <c r="C52" s="71"/>
+      <c r="A52" s="91"/>
+      <c r="B52" s="91"/>
+      <c r="C52" s="95"/>
       <c r="D52" s="24">
         <v>3</v>
       </c>
@@ -6415,9 +6415,9 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="72"/>
-      <c r="B53" s="72"/>
-      <c r="C53" s="71"/>
+      <c r="A53" s="91"/>
+      <c r="B53" s="91"/>
+      <c r="C53" s="95"/>
       <c r="D53" s="24">
         <v>4</v>
       </c>
@@ -6426,9 +6426,9 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="72"/>
-      <c r="B54" s="72"/>
-      <c r="C54" s="71"/>
+      <c r="A54" s="91"/>
+      <c r="B54" s="91"/>
+      <c r="C54" s="95"/>
       <c r="D54" s="24">
         <v>5</v>
       </c>
@@ -6437,9 +6437,9 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="72"/>
-      <c r="B55" s="72"/>
-      <c r="C55" s="71"/>
+      <c r="A55" s="91"/>
+      <c r="B55" s="91"/>
+      <c r="C55" s="95"/>
       <c r="D55" s="24">
         <v>6</v>
       </c>
@@ -6448,9 +6448,9 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="72"/>
-      <c r="B56" s="72"/>
-      <c r="C56" s="71"/>
+      <c r="A56" s="91"/>
+      <c r="B56" s="91"/>
+      <c r="C56" s="95"/>
       <c r="D56" s="24">
         <v>7</v>
       </c>
@@ -6459,13 +6459,13 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="72" t="s">
+      <c r="A57" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="B57" s="72" t="s">
+      <c r="B57" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="71">
+      <c r="C57" s="95">
         <v>8</v>
       </c>
       <c r="D57" s="24">
@@ -6476,9 +6476,9 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="72"/>
-      <c r="B58" s="72"/>
-      <c r="C58" s="71"/>
+      <c r="A58" s="91"/>
+      <c r="B58" s="91"/>
+      <c r="C58" s="95"/>
       <c r="D58" s="24">
         <v>2</v>
       </c>
@@ -6487,9 +6487,9 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="72"/>
-      <c r="B59" s="72"/>
-      <c r="C59" s="71"/>
+      <c r="A59" s="91"/>
+      <c r="B59" s="91"/>
+      <c r="C59" s="95"/>
       <c r="D59" s="24">
         <v>3</v>
       </c>
@@ -6498,9 +6498,9 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="72"/>
-      <c r="B60" s="72"/>
-      <c r="C60" s="71"/>
+      <c r="A60" s="91"/>
+      <c r="B60" s="91"/>
+      <c r="C60" s="95"/>
       <c r="D60" s="24">
         <v>4</v>
       </c>
@@ -6509,9 +6509,9 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="72"/>
-      <c r="B61" s="72"/>
-      <c r="C61" s="71"/>
+      <c r="A61" s="91"/>
+      <c r="B61" s="91"/>
+      <c r="C61" s="95"/>
       <c r="D61" s="24">
         <v>5</v>
       </c>
@@ -6520,9 +6520,9 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="72"/>
-      <c r="B62" s="72"/>
-      <c r="C62" s="71"/>
+      <c r="A62" s="91"/>
+      <c r="B62" s="91"/>
+      <c r="C62" s="95"/>
       <c r="D62" s="24">
         <v>6</v>
       </c>
@@ -6531,9 +6531,9 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="72"/>
-      <c r="B63" s="72"/>
-      <c r="C63" s="71"/>
+      <c r="A63" s="91"/>
+      <c r="B63" s="91"/>
+      <c r="C63" s="95"/>
       <c r="D63" s="24">
         <v>7</v>
       </c>
@@ -6542,9 +6542,9 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="72"/>
-      <c r="B64" s="72"/>
-      <c r="C64" s="71"/>
+      <c r="A64" s="91"/>
+      <c r="B64" s="91"/>
+      <c r="C64" s="95"/>
       <c r="D64" s="24">
         <v>8</v>
       </c>
@@ -6553,13 +6553,13 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="72" t="s">
+      <c r="A65" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="B65" s="72" t="s">
+      <c r="B65" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="C65" s="71">
+      <c r="C65" s="95">
         <v>2</v>
       </c>
       <c r="D65" s="24">
@@ -6570,9 +6570,9 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="72"/>
-      <c r="B66" s="72"/>
-      <c r="C66" s="71"/>
+      <c r="A66" s="91"/>
+      <c r="B66" s="91"/>
+      <c r="C66" s="95"/>
       <c r="D66" s="24">
         <v>2</v>
       </c>
@@ -6598,13 +6598,13 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="72" t="s">
+      <c r="A68" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="72" t="s">
+      <c r="B68" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="C68" s="71">
+      <c r="C68" s="95">
         <v>3</v>
       </c>
       <c r="D68" s="24">
@@ -6615,9 +6615,9 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="72"/>
-      <c r="B69" s="72"/>
-      <c r="C69" s="71"/>
+      <c r="A69" s="91"/>
+      <c r="B69" s="91"/>
+      <c r="C69" s="95"/>
       <c r="D69" s="24">
         <v>2</v>
       </c>
@@ -6626,9 +6626,9 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="72"/>
-      <c r="B70" s="72"/>
-      <c r="C70" s="71"/>
+      <c r="A70" s="91"/>
+      <c r="B70" s="91"/>
+      <c r="C70" s="95"/>
       <c r="D70" s="24">
         <v>3</v>
       </c>
@@ -6637,13 +6637,13 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="72" t="s">
+      <c r="A71" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="B71" s="72" t="s">
+      <c r="B71" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="C71" s="71">
+      <c r="C71" s="95">
         <v>44</v>
       </c>
       <c r="D71" s="24">
@@ -6654,9 +6654,9 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="72"/>
-      <c r="B72" s="72"/>
-      <c r="C72" s="71"/>
+      <c r="A72" s="91"/>
+      <c r="B72" s="91"/>
+      <c r="C72" s="95"/>
       <c r="D72" s="24">
         <v>2</v>
       </c>
@@ -6665,9 +6665,9 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="72"/>
-      <c r="B73" s="72"/>
-      <c r="C73" s="71"/>
+      <c r="A73" s="91"/>
+      <c r="B73" s="91"/>
+      <c r="C73" s="95"/>
       <c r="D73" s="24">
         <v>3</v>
       </c>
@@ -6676,9 +6676,9 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="72"/>
-      <c r="B74" s="72"/>
-      <c r="C74" s="71"/>
+      <c r="A74" s="91"/>
+      <c r="B74" s="91"/>
+      <c r="C74" s="95"/>
       <c r="D74" s="24">
         <v>4</v>
       </c>
@@ -6687,9 +6687,9 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="72"/>
-      <c r="B75" s="72"/>
-      <c r="C75" s="71"/>
+      <c r="A75" s="91"/>
+      <c r="B75" s="91"/>
+      <c r="C75" s="95"/>
       <c r="D75" s="24">
         <v>5</v>
       </c>
@@ -6698,9 +6698,9 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="72"/>
-      <c r="B76" s="72"/>
-      <c r="C76" s="71"/>
+      <c r="A76" s="91"/>
+      <c r="B76" s="91"/>
+      <c r="C76" s="95"/>
       <c r="D76" s="24">
         <v>6</v>
       </c>
@@ -6709,9 +6709,9 @@
       </c>
     </row>
     <row r="77" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="72"/>
-      <c r="B77" s="72"/>
-      <c r="C77" s="71"/>
+      <c r="A77" s="91"/>
+      <c r="B77" s="91"/>
+      <c r="C77" s="95"/>
       <c r="D77" s="24">
         <v>7</v>
       </c>
@@ -6720,9 +6720,9 @@
       </c>
     </row>
     <row r="78" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="72"/>
-      <c r="B78" s="72"/>
-      <c r="C78" s="71"/>
+      <c r="A78" s="91"/>
+      <c r="B78" s="91"/>
+      <c r="C78" s="95"/>
       <c r="D78" s="24">
         <v>8</v>
       </c>
@@ -6731,9 +6731,9 @@
       </c>
     </row>
     <row r="79" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="72"/>
-      <c r="B79" s="72"/>
-      <c r="C79" s="71"/>
+      <c r="A79" s="91"/>
+      <c r="B79" s="91"/>
+      <c r="C79" s="95"/>
       <c r="D79" s="24">
         <v>9</v>
       </c>
@@ -6742,9 +6742,9 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="72"/>
-      <c r="B80" s="72"/>
-      <c r="C80" s="71"/>
+      <c r="A80" s="91"/>
+      <c r="B80" s="91"/>
+      <c r="C80" s="95"/>
       <c r="D80" s="24">
         <v>10</v>
       </c>
@@ -6753,9 +6753,9 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="72"/>
-      <c r="B81" s="72"/>
-      <c r="C81" s="71"/>
+      <c r="A81" s="91"/>
+      <c r="B81" s="91"/>
+      <c r="C81" s="95"/>
       <c r="D81" s="24">
         <v>11</v>
       </c>
@@ -6764,9 +6764,9 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="72"/>
-      <c r="B82" s="72"/>
-      <c r="C82" s="71"/>
+      <c r="A82" s="91"/>
+      <c r="B82" s="91"/>
+      <c r="C82" s="95"/>
       <c r="D82" s="24">
         <v>12</v>
       </c>
@@ -6775,9 +6775,9 @@
       </c>
     </row>
     <row r="83" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="72"/>
-      <c r="B83" s="72"/>
-      <c r="C83" s="71"/>
+      <c r="A83" s="91"/>
+      <c r="B83" s="91"/>
+      <c r="C83" s="95"/>
       <c r="D83" s="24">
         <v>13</v>
       </c>
@@ -6786,9 +6786,9 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="72"/>
-      <c r="B84" s="72"/>
-      <c r="C84" s="71"/>
+      <c r="A84" s="91"/>
+      <c r="B84" s="91"/>
+      <c r="C84" s="95"/>
       <c r="D84" s="24">
         <v>14</v>
       </c>
@@ -6797,9 +6797,9 @@
       </c>
     </row>
     <row r="85" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="72"/>
-      <c r="B85" s="72"/>
-      <c r="C85" s="71"/>
+      <c r="A85" s="91"/>
+      <c r="B85" s="91"/>
+      <c r="C85" s="95"/>
       <c r="D85" s="24">
         <v>15</v>
       </c>
@@ -6808,9 +6808,9 @@
       </c>
     </row>
     <row r="86" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="72"/>
-      <c r="B86" s="72"/>
-      <c r="C86" s="71"/>
+      <c r="A86" s="91"/>
+      <c r="B86" s="91"/>
+      <c r="C86" s="95"/>
       <c r="D86" s="24">
         <v>16</v>
       </c>
@@ -6819,9 +6819,9 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="72"/>
-      <c r="B87" s="72"/>
-      <c r="C87" s="71"/>
+      <c r="A87" s="91"/>
+      <c r="B87" s="91"/>
+      <c r="C87" s="95"/>
       <c r="D87" s="24">
         <v>17</v>
       </c>
@@ -6830,9 +6830,9 @@
       </c>
     </row>
     <row r="88" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="72"/>
-      <c r="B88" s="72"/>
-      <c r="C88" s="71"/>
+      <c r="A88" s="91"/>
+      <c r="B88" s="91"/>
+      <c r="C88" s="95"/>
       <c r="D88" s="24">
         <v>18</v>
       </c>
@@ -6841,9 +6841,9 @@
       </c>
     </row>
     <row r="89" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="72"/>
-      <c r="B89" s="72"/>
-      <c r="C89" s="71"/>
+      <c r="A89" s="91"/>
+      <c r="B89" s="91"/>
+      <c r="C89" s="95"/>
       <c r="D89" s="24">
         <v>19</v>
       </c>
@@ -6852,9 +6852,9 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="72"/>
-      <c r="B90" s="72"/>
-      <c r="C90" s="71"/>
+      <c r="A90" s="91"/>
+      <c r="B90" s="91"/>
+      <c r="C90" s="95"/>
       <c r="D90" s="24">
         <v>20</v>
       </c>
@@ -6863,9 +6863,9 @@
       </c>
     </row>
     <row r="91" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="72"/>
-      <c r="B91" s="72"/>
-      <c r="C91" s="71"/>
+      <c r="A91" s="91"/>
+      <c r="B91" s="91"/>
+      <c r="C91" s="95"/>
       <c r="D91" s="24">
         <v>21</v>
       </c>
@@ -6874,9 +6874,9 @@
       </c>
     </row>
     <row r="92" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="72"/>
-      <c r="B92" s="72"/>
-      <c r="C92" s="71"/>
+      <c r="A92" s="91"/>
+      <c r="B92" s="91"/>
+      <c r="C92" s="95"/>
       <c r="D92" s="24">
         <v>22</v>
       </c>
@@ -6885,9 +6885,9 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="72"/>
-      <c r="B93" s="72"/>
-      <c r="C93" s="71"/>
+      <c r="A93" s="91"/>
+      <c r="B93" s="91"/>
+      <c r="C93" s="95"/>
       <c r="D93" s="24">
         <v>23</v>
       </c>
@@ -6896,9 +6896,9 @@
       </c>
     </row>
     <row r="94" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="72"/>
-      <c r="B94" s="72"/>
-      <c r="C94" s="71"/>
+      <c r="A94" s="91"/>
+      <c r="B94" s="91"/>
+      <c r="C94" s="95"/>
       <c r="D94" s="24">
         <v>24</v>
       </c>
@@ -6907,9 +6907,9 @@
       </c>
     </row>
     <row r="95" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="72"/>
-      <c r="B95" s="72"/>
-      <c r="C95" s="71"/>
+      <c r="A95" s="91"/>
+      <c r="B95" s="91"/>
+      <c r="C95" s="95"/>
       <c r="D95" s="24">
         <v>25</v>
       </c>
@@ -6918,9 +6918,9 @@
       </c>
     </row>
     <row r="96" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="72"/>
-      <c r="B96" s="72"/>
-      <c r="C96" s="71"/>
+      <c r="A96" s="91"/>
+      <c r="B96" s="91"/>
+      <c r="C96" s="95"/>
       <c r="D96" s="24">
         <v>26</v>
       </c>
@@ -6929,9 +6929,9 @@
       </c>
     </row>
     <row r="97" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="72"/>
-      <c r="B97" s="72"/>
-      <c r="C97" s="71"/>
+      <c r="A97" s="91"/>
+      <c r="B97" s="91"/>
+      <c r="C97" s="95"/>
       <c r="D97" s="24">
         <v>27</v>
       </c>
@@ -6940,9 +6940,9 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="72"/>
-      <c r="B98" s="72"/>
-      <c r="C98" s="71"/>
+      <c r="A98" s="91"/>
+      <c r="B98" s="91"/>
+      <c r="C98" s="95"/>
       <c r="D98" s="24">
         <v>28</v>
       </c>
@@ -6951,9 +6951,9 @@
       </c>
     </row>
     <row r="99" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="72"/>
-      <c r="B99" s="72"/>
-      <c r="C99" s="71"/>
+      <c r="A99" s="91"/>
+      <c r="B99" s="91"/>
+      <c r="C99" s="95"/>
       <c r="D99" s="24">
         <v>29</v>
       </c>
@@ -6962,9 +6962,9 @@
       </c>
     </row>
     <row r="100" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="72"/>
-      <c r="B100" s="72"/>
-      <c r="C100" s="71"/>
+      <c r="A100" s="91"/>
+      <c r="B100" s="91"/>
+      <c r="C100" s="95"/>
       <c r="D100" s="24">
         <v>30</v>
       </c>
@@ -6973,9 +6973,9 @@
       </c>
     </row>
     <row r="101" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="72"/>
-      <c r="B101" s="72"/>
-      <c r="C101" s="71"/>
+      <c r="A101" s="91"/>
+      <c r="B101" s="91"/>
+      <c r="C101" s="95"/>
       <c r="D101" s="24">
         <v>31</v>
       </c>
@@ -6984,9 +6984,9 @@
       </c>
     </row>
     <row r="102" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="72"/>
-      <c r="B102" s="72"/>
-      <c r="C102" s="71"/>
+      <c r="A102" s="91"/>
+      <c r="B102" s="91"/>
+      <c r="C102" s="95"/>
       <c r="D102" s="24">
         <v>32</v>
       </c>
@@ -6995,9 +6995,9 @@
       </c>
     </row>
     <row r="103" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="72"/>
-      <c r="B103" s="72"/>
-      <c r="C103" s="71"/>
+      <c r="A103" s="91"/>
+      <c r="B103" s="91"/>
+      <c r="C103" s="95"/>
       <c r="D103" s="24">
         <v>33</v>
       </c>
@@ -7006,9 +7006,9 @@
       </c>
     </row>
     <row r="104" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="72"/>
-      <c r="B104" s="72"/>
-      <c r="C104" s="71"/>
+      <c r="A104" s="91"/>
+      <c r="B104" s="91"/>
+      <c r="C104" s="95"/>
       <c r="D104" s="24">
         <v>34</v>
       </c>
@@ -7017,9 +7017,9 @@
       </c>
     </row>
     <row r="105" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="72"/>
-      <c r="B105" s="72"/>
-      <c r="C105" s="71"/>
+      <c r="A105" s="91"/>
+      <c r="B105" s="91"/>
+      <c r="C105" s="95"/>
       <c r="D105" s="24">
         <v>35</v>
       </c>
@@ -7028,9 +7028,9 @@
       </c>
     </row>
     <row r="106" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="72"/>
-      <c r="B106" s="72"/>
-      <c r="C106" s="71"/>
+      <c r="A106" s="91"/>
+      <c r="B106" s="91"/>
+      <c r="C106" s="95"/>
       <c r="D106" s="24">
         <v>36</v>
       </c>
@@ -7039,9 +7039,9 @@
       </c>
     </row>
     <row r="107" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="72"/>
-      <c r="B107" s="72"/>
-      <c r="C107" s="71"/>
+      <c r="A107" s="91"/>
+      <c r="B107" s="91"/>
+      <c r="C107" s="95"/>
       <c r="D107" s="24">
         <v>37</v>
       </c>
@@ -7050,9 +7050,9 @@
       </c>
     </row>
     <row r="108" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="72"/>
-      <c r="B108" s="72"/>
-      <c r="C108" s="71"/>
+      <c r="A108" s="91"/>
+      <c r="B108" s="91"/>
+      <c r="C108" s="95"/>
       <c r="D108" s="24">
         <v>38</v>
       </c>
@@ -7061,9 +7061,9 @@
       </c>
     </row>
     <row r="109" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="72"/>
-      <c r="B109" s="72"/>
-      <c r="C109" s="71"/>
+      <c r="A109" s="91"/>
+      <c r="B109" s="91"/>
+      <c r="C109" s="95"/>
       <c r="D109" s="24">
         <v>39</v>
       </c>
@@ -7072,9 +7072,9 @@
       </c>
     </row>
     <row r="110" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="72"/>
-      <c r="B110" s="72"/>
-      <c r="C110" s="71"/>
+      <c r="A110" s="91"/>
+      <c r="B110" s="91"/>
+      <c r="C110" s="95"/>
       <c r="D110" s="24">
         <v>40</v>
       </c>
@@ -7083,9 +7083,9 @@
       </c>
     </row>
     <row r="111" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="72"/>
-      <c r="B111" s="72"/>
-      <c r="C111" s="71"/>
+      <c r="A111" s="91"/>
+      <c r="B111" s="91"/>
+      <c r="C111" s="95"/>
       <c r="D111" s="24">
         <v>41</v>
       </c>
@@ -7094,9 +7094,9 @@
       </c>
     </row>
     <row r="112" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="72"/>
-      <c r="B112" s="72"/>
-      <c r="C112" s="71"/>
+      <c r="A112" s="91"/>
+      <c r="B112" s="91"/>
+      <c r="C112" s="95"/>
       <c r="D112" s="24">
         <v>42</v>
       </c>
@@ -7105,9 +7105,9 @@
       </c>
     </row>
     <row r="113" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="72"/>
-      <c r="B113" s="72"/>
-      <c r="C113" s="71"/>
+      <c r="A113" s="91"/>
+      <c r="B113" s="91"/>
+      <c r="C113" s="95"/>
       <c r="D113" s="24">
         <v>43</v>
       </c>
@@ -7116,9 +7116,9 @@
       </c>
     </row>
     <row r="114" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="72"/>
-      <c r="B114" s="72"/>
-      <c r="C114" s="71"/>
+      <c r="A114" s="91"/>
+      <c r="B114" s="91"/>
+      <c r="C114" s="95"/>
       <c r="D114" s="24">
         <v>44</v>
       </c>
@@ -7127,13 +7127,13 @@
       </c>
     </row>
     <row r="115" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="72" t="s">
+      <c r="A115" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="B115" s="72" t="s">
+      <c r="B115" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="C115" s="71">
+      <c r="C115" s="95">
         <v>5</v>
       </c>
       <c r="D115" s="24">
@@ -7144,9 +7144,9 @@
       </c>
     </row>
     <row r="116" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="72"/>
-      <c r="B116" s="72"/>
-      <c r="C116" s="71"/>
+      <c r="A116" s="91"/>
+      <c r="B116" s="91"/>
+      <c r="C116" s="95"/>
       <c r="D116" s="24">
         <v>2</v>
       </c>
@@ -7155,9 +7155,9 @@
       </c>
     </row>
     <row r="117" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="72"/>
-      <c r="B117" s="72"/>
-      <c r="C117" s="71"/>
+      <c r="A117" s="91"/>
+      <c r="B117" s="91"/>
+      <c r="C117" s="95"/>
       <c r="D117" s="24">
         <v>3</v>
       </c>
@@ -7166,9 +7166,9 @@
       </c>
     </row>
     <row r="118" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="72"/>
-      <c r="B118" s="72"/>
-      <c r="C118" s="71"/>
+      <c r="A118" s="91"/>
+      <c r="B118" s="91"/>
+      <c r="C118" s="95"/>
       <c r="D118" s="24">
         <v>4</v>
       </c>
@@ -7177,9 +7177,9 @@
       </c>
     </row>
     <row r="119" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="72"/>
-      <c r="B119" s="72"/>
-      <c r="C119" s="71"/>
+      <c r="A119" s="91"/>
+      <c r="B119" s="91"/>
+      <c r="C119" s="95"/>
       <c r="D119" s="24">
         <v>5</v>
       </c>
@@ -7188,13 +7188,13 @@
       </c>
     </row>
     <row r="120" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="72" t="s">
+      <c r="A120" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="B120" s="72" t="s">
+      <c r="B120" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="C120" s="71">
+      <c r="C120" s="95">
         <v>4</v>
       </c>
       <c r="D120" s="24">
@@ -7205,9 +7205,9 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="72"/>
-      <c r="B121" s="72"/>
-      <c r="C121" s="71"/>
+      <c r="A121" s="91"/>
+      <c r="B121" s="91"/>
+      <c r="C121" s="95"/>
       <c r="D121" s="24">
         <v>2</v>
       </c>
@@ -7216,9 +7216,9 @@
       </c>
     </row>
     <row r="122" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="72"/>
-      <c r="B122" s="72"/>
-      <c r="C122" s="71"/>
+      <c r="A122" s="91"/>
+      <c r="B122" s="91"/>
+      <c r="C122" s="95"/>
       <c r="D122" s="24">
         <v>3</v>
       </c>
@@ -7227,9 +7227,9 @@
       </c>
     </row>
     <row r="123" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="72"/>
-      <c r="B123" s="72"/>
-      <c r="C123" s="71"/>
+      <c r="A123" s="91"/>
+      <c r="B123" s="91"/>
+      <c r="C123" s="95"/>
       <c r="D123" s="24">
         <v>4</v>
       </c>
@@ -7238,13 +7238,13 @@
       </c>
     </row>
     <row r="124" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="72" t="s">
+      <c r="A124" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="B124" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="C124" s="71">
+      <c r="B124" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" s="95">
         <v>2</v>
       </c>
       <c r="D124" s="24">
@@ -7255,9 +7255,9 @@
       </c>
     </row>
     <row r="125" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="72"/>
-      <c r="B125" s="72"/>
-      <c r="C125" s="71"/>
+      <c r="A125" s="91"/>
+      <c r="B125" s="91"/>
+      <c r="C125" s="95"/>
       <c r="D125" s="24">
         <v>2</v>
       </c>
@@ -7266,13 +7266,13 @@
       </c>
     </row>
     <row r="126" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="72" t="s">
+      <c r="A126" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="B126" s="72" t="s">
+      <c r="B126" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="C126" s="71">
+      <c r="C126" s="95">
         <v>2</v>
       </c>
       <c r="D126" s="24">
@@ -7283,9 +7283,9 @@
       </c>
     </row>
     <row r="127" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="72"/>
-      <c r="B127" s="72"/>
-      <c r="C127" s="71"/>
+      <c r="A127" s="91"/>
+      <c r="B127" s="91"/>
+      <c r="C127" s="95"/>
       <c r="D127" s="24">
         <v>1</v>
       </c>
@@ -7298,6 +7298,35 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C57:C64"/>
+    <mergeCell ref="C50:C56"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="C115:C119"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="C71:C114"/>
+    <mergeCell ref="A71:A114"/>
+    <mergeCell ref="B71:B114"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="B50:B56"/>
+    <mergeCell ref="A57:A64"/>
+    <mergeCell ref="B57:B64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="A115:A119"/>
+    <mergeCell ref="B115:B119"/>
+    <mergeCell ref="A120:A123"/>
+    <mergeCell ref="B120:B123"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="A1:B1"/>
@@ -7314,35 +7343,6 @@
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="A115:A119"/>
-    <mergeCell ref="B115:B119"/>
-    <mergeCell ref="A120:A123"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="A71:A114"/>
-    <mergeCell ref="B71:B114"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="A50:A56"/>
-    <mergeCell ref="B50:B56"/>
-    <mergeCell ref="A57:A64"/>
-    <mergeCell ref="B57:B64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="C115:C119"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="C71:C114"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C57:C64"/>
-    <mergeCell ref="C50:C56"/>
-    <mergeCell ref="C48:C49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7367,19 +7367,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="76" t="s">
+      <c r="B1" s="92"/>
+      <c r="C1" s="96" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
@@ -7388,7 +7388,7 @@
       <c r="B2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="76"/>
+      <c r="C2" s="96"/>
       <c r="D2" s="23" t="s">
         <v>51</v>
       </c>
@@ -7832,21 +7832,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="40" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="74" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
     </row>
     <row r="2" spans="1:12" s="40" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -7855,7 +7855,7 @@
       <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="93"/>
       <c r="D2" s="12" t="s">
         <v>51</v>
       </c>
@@ -8085,13 +8085,13 @@
       <c r="L9" s="34"/>
     </row>
     <row r="10" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="78" t="s">
+      <c r="B10" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="77">
+      <c r="C10" s="97">
         <v>2</v>
       </c>
       <c r="D10" s="20">
@@ -8115,9 +8115,9 @@
       <c r="L10" s="34"/>
     </row>
     <row r="11" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="77"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="20">
         <v>2</v>
       </c>
@@ -8140,13 +8140,13 @@
       <c r="L11" s="34"/>
     </row>
     <row r="12" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="77">
+      <c r="C12" s="97">
         <v>3</v>
       </c>
       <c r="D12" s="20">
@@ -8170,9 +8170,9 @@
       <c r="L12" s="34"/>
     </row>
     <row r="13" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="78"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="77"/>
+      <c r="A13" s="98"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="20">
         <v>2</v>
       </c>
@@ -8194,9 +8194,9 @@
       <c r="L13" s="34"/>
     </row>
     <row r="14" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="78"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="77"/>
+      <c r="A14" s="98"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="97"/>
       <c r="D14" s="20">
         <v>3</v>
       </c>
@@ -8372,10 +8372,10 @@
       <c r="A20" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="78" t="s">
+      <c r="B20" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="77">
+      <c r="C20" s="97">
         <v>0</v>
       </c>
       <c r="D20" s="20">
@@ -8400,8 +8400,8 @@
     </row>
     <row r="21" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
-      <c r="B21" s="78"/>
-      <c r="C21" s="77"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="97"/>
       <c r="D21" s="20">
         <v>2</v>
       </c>
@@ -8424,8 +8424,8 @@
     </row>
     <row r="22" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
-      <c r="B22" s="78"/>
-      <c r="C22" s="77"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="97"/>
       <c r="D22" s="20">
         <v>3</v>
       </c>
@@ -8448,8 +8448,8 @@
     </row>
     <row r="23" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
-      <c r="B23" s="78"/>
-      <c r="C23" s="77"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="97"/>
       <c r="D23" s="20">
         <v>4</v>
       </c>
@@ -8534,17 +8534,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C14"/>
     <mergeCell ref="C20:C23"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8568,20 +8568,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="80" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="100" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
@@ -8590,7 +8590,7 @@
       <c r="B2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="80"/>
+      <c r="C2" s="100"/>
       <c r="D2" s="39" t="s">
         <v>51</v>
       </c>
@@ -8608,13 +8608,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="77">
+      <c r="C3" s="97">
         <v>0</v>
       </c>
       <c r="D3" s="20">
@@ -8634,9 +8634,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="81"/>
-      <c r="B4" s="81"/>
-      <c r="C4" s="77"/>
+      <c r="A4" s="101"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="97"/>
       <c r="D4" s="20">
         <v>2</v>
       </c>
@@ -8654,9 +8654,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="81"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="77"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="97"/>
       <c r="D5" s="20">
         <v>3</v>
       </c>
@@ -8960,13 +8960,13 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="77">
+      <c r="C17" s="97">
         <v>36</v>
       </c>
       <c r="D17" s="20">
@@ -8986,9 +8986,9 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="81"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="77"/>
+      <c r="A18" s="101"/>
+      <c r="B18" s="101"/>
+      <c r="C18" s="97"/>
       <c r="D18" s="20">
         <v>2</v>
       </c>
@@ -9006,9 +9006,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="81"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="77"/>
+      <c r="A19" s="101"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="97"/>
       <c r="D19" s="20">
         <v>3</v>
       </c>
@@ -9026,9 +9026,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="81"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="77"/>
+      <c r="A20" s="101"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="97"/>
       <c r="D20" s="20">
         <v>4</v>
       </c>
@@ -9046,9 +9046,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="81"/>
-      <c r="B21" s="81"/>
-      <c r="C21" s="77"/>
+      <c r="A21" s="101"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="97"/>
       <c r="D21" s="20">
         <v>5</v>
       </c>
@@ -9066,9 +9066,9 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="81"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="77"/>
+      <c r="A22" s="101"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="97"/>
       <c r="D22" s="20">
         <v>6</v>
       </c>
@@ -9086,9 +9086,9 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="81"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="77"/>
+      <c r="A23" s="101"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="97"/>
       <c r="D23" s="20">
         <v>7</v>
       </c>
@@ -9106,9 +9106,9 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="81"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="77"/>
+      <c r="A24" s="101"/>
+      <c r="B24" s="101"/>
+      <c r="C24" s="97"/>
       <c r="D24" s="20">
         <v>8</v>
       </c>
@@ -9126,9 +9126,9 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="81"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="77"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="97"/>
       <c r="D25" s="20">
         <v>9</v>
       </c>
@@ -9146,9 +9146,9 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="81"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="77"/>
+      <c r="A26" s="101"/>
+      <c r="B26" s="101"/>
+      <c r="C26" s="97"/>
       <c r="D26" s="20">
         <v>10</v>
       </c>
@@ -9166,9 +9166,9 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="81"/>
-      <c r="B27" s="81"/>
-      <c r="C27" s="77"/>
+      <c r="A27" s="101"/>
+      <c r="B27" s="101"/>
+      <c r="C27" s="97"/>
       <c r="D27" s="20">
         <v>11</v>
       </c>
@@ -9186,9 +9186,9 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="81"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="77"/>
+      <c r="A28" s="101"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="97"/>
       <c r="D28" s="20">
         <v>12</v>
       </c>
@@ -9206,9 +9206,9 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="81"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="77"/>
+      <c r="A29" s="101"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="97"/>
       <c r="D29" s="20">
         <v>13</v>
       </c>
@@ -9226,9 +9226,9 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="81"/>
-      <c r="B30" s="81"/>
-      <c r="C30" s="77"/>
+      <c r="A30" s="101"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="97"/>
       <c r="D30" s="20">
         <v>14</v>
       </c>
@@ -9246,9 +9246,9 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="81"/>
-      <c r="B31" s="81"/>
-      <c r="C31" s="77"/>
+      <c r="A31" s="101"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="97"/>
       <c r="D31" s="20">
         <v>15</v>
       </c>
@@ -9266,9 +9266,9 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="81"/>
-      <c r="B32" s="81"/>
-      <c r="C32" s="77"/>
+      <c r="A32" s="101"/>
+      <c r="B32" s="101"/>
+      <c r="C32" s="97"/>
       <c r="D32" s="20">
         <v>16</v>
       </c>
@@ -9286,9 +9286,9 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="81"/>
-      <c r="B33" s="81"/>
-      <c r="C33" s="77"/>
+      <c r="A33" s="101"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="97"/>
       <c r="D33" s="20">
         <v>17</v>
       </c>
@@ -9306,9 +9306,9 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="81"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="77"/>
+      <c r="A34" s="101"/>
+      <c r="B34" s="101"/>
+      <c r="C34" s="97"/>
       <c r="D34" s="20">
         <v>18</v>
       </c>
@@ -9326,9 +9326,9 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="81"/>
-      <c r="B35" s="81"/>
-      <c r="C35" s="77"/>
+      <c r="A35" s="101"/>
+      <c r="B35" s="101"/>
+      <c r="C35" s="97"/>
       <c r="D35" s="20">
         <v>19</v>
       </c>
@@ -9346,9 +9346,9 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="81"/>
-      <c r="B36" s="81"/>
-      <c r="C36" s="77"/>
+      <c r="A36" s="101"/>
+      <c r="B36" s="101"/>
+      <c r="C36" s="97"/>
       <c r="D36" s="20">
         <v>20</v>
       </c>
@@ -9366,9 +9366,9 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="81"/>
-      <c r="B37" s="81"/>
-      <c r="C37" s="77"/>
+      <c r="A37" s="101"/>
+      <c r="B37" s="101"/>
+      <c r="C37" s="97"/>
       <c r="D37" s="20">
         <v>21</v>
       </c>
@@ -9386,9 +9386,9 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="81"/>
-      <c r="B38" s="81"/>
-      <c r="C38" s="77"/>
+      <c r="A38" s="101"/>
+      <c r="B38" s="101"/>
+      <c r="C38" s="97"/>
       <c r="D38" s="20">
         <v>22</v>
       </c>
@@ -9406,9 +9406,9 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="81"/>
-      <c r="B39" s="81"/>
-      <c r="C39" s="77"/>
+      <c r="A39" s="101"/>
+      <c r="B39" s="101"/>
+      <c r="C39" s="97"/>
       <c r="D39" s="20">
         <v>23</v>
       </c>
@@ -9426,9 +9426,9 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="81"/>
-      <c r="B40" s="81"/>
-      <c r="C40" s="77"/>
+      <c r="A40" s="101"/>
+      <c r="B40" s="101"/>
+      <c r="C40" s="97"/>
       <c r="D40" s="20">
         <v>24</v>
       </c>
@@ -9446,9 +9446,9 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="81"/>
-      <c r="B41" s="81"/>
-      <c r="C41" s="77"/>
+      <c r="A41" s="101"/>
+      <c r="B41" s="101"/>
+      <c r="C41" s="97"/>
       <c r="D41" s="20">
         <v>25</v>
       </c>
@@ -9466,9 +9466,9 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="81"/>
-      <c r="B42" s="81"/>
-      <c r="C42" s="77"/>
+      <c r="A42" s="101"/>
+      <c r="B42" s="101"/>
+      <c r="C42" s="97"/>
       <c r="D42" s="20">
         <v>26</v>
       </c>
@@ -9486,9 +9486,9 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="81"/>
-      <c r="B43" s="81"/>
-      <c r="C43" s="77"/>
+      <c r="A43" s="101"/>
+      <c r="B43" s="101"/>
+      <c r="C43" s="97"/>
       <c r="D43" s="20">
         <v>27</v>
       </c>
@@ -9506,9 +9506,9 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="81"/>
-      <c r="B44" s="81"/>
-      <c r="C44" s="77"/>
+      <c r="A44" s="101"/>
+      <c r="B44" s="101"/>
+      <c r="C44" s="97"/>
       <c r="D44" s="20">
         <v>28</v>
       </c>
@@ -9526,9 +9526,9 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="81"/>
-      <c r="B45" s="81"/>
-      <c r="C45" s="77"/>
+      <c r="A45" s="101"/>
+      <c r="B45" s="101"/>
+      <c r="C45" s="97"/>
       <c r="D45" s="20">
         <v>29</v>
       </c>
@@ -9546,9 +9546,9 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="81"/>
-      <c r="B46" s="81"/>
-      <c r="C46" s="77"/>
+      <c r="A46" s="101"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="97"/>
       <c r="D46" s="20">
         <v>30</v>
       </c>
@@ -9566,9 +9566,9 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="81"/>
-      <c r="B47" s="81"/>
-      <c r="C47" s="77"/>
+      <c r="A47" s="101"/>
+      <c r="B47" s="101"/>
+      <c r="C47" s="97"/>
       <c r="D47" s="20">
         <v>31</v>
       </c>
@@ -9586,9 +9586,9 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="81"/>
-      <c r="B48" s="81"/>
-      <c r="C48" s="77"/>
+      <c r="A48" s="101"/>
+      <c r="B48" s="101"/>
+      <c r="C48" s="97"/>
       <c r="D48" s="20">
         <v>32</v>
       </c>
@@ -9606,9 +9606,9 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="81"/>
-      <c r="B49" s="81"/>
-      <c r="C49" s="77"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="97"/>
       <c r="D49" s="20">
         <v>33</v>
       </c>
@@ -9626,9 +9626,9 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="81"/>
-      <c r="B50" s="81"/>
-      <c r="C50" s="77"/>
+      <c r="A50" s="101"/>
+      <c r="B50" s="101"/>
+      <c r="C50" s="97"/>
       <c r="D50" s="20">
         <v>34</v>
       </c>
@@ -9646,9 +9646,9 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="81"/>
-      <c r="B51" s="81"/>
-      <c r="C51" s="77"/>
+      <c r="A51" s="101"/>
+      <c r="B51" s="101"/>
+      <c r="C51" s="97"/>
       <c r="D51" s="20">
         <v>35</v>
       </c>
@@ -9666,9 +9666,9 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="81"/>
-      <c r="B52" s="81"/>
-      <c r="C52" s="77"/>
+      <c r="A52" s="101"/>
+      <c r="B52" s="101"/>
+      <c r="C52" s="97"/>
       <c r="D52" s="20">
         <v>36</v>
       </c>
@@ -9835,36 +9835,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="74" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
     </row>
     <row r="2" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -9873,7 +9873,7 @@
       <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="93"/>
       <c r="D2" s="12" t="s">
         <v>51</v>
       </c>
@@ -10863,13 +10863,13 @@
       <c r="AA14" s="3"/>
     </row>
     <row r="15" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="71">
+      <c r="C15" s="95">
         <v>0</v>
       </c>
       <c r="D15" s="3">
@@ -10940,9 +10940,9 @@
       <c r="AA15" s="3"/>
     </row>
     <row r="16" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="78"/>
-      <c r="B16" s="78"/>
-      <c r="C16" s="71"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="95"/>
       <c r="D16" s="3">
         <v>2</v>
       </c>
@@ -11575,38 +11575,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="74" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="69"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
     </row>
     <row r="2" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -11615,7 +11615,7 @@
       <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="93"/>
       <c r="D2" s="12" t="s">
         <v>51</v>
       </c>
@@ -13078,43 +13078,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="74" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
+      <c r="AA1" s="86"/>
+      <c r="AB1" s="86"/>
+      <c r="AC1" s="86"/>
+      <c r="AD1" s="86"/>
+      <c r="AE1" s="86"/>
     </row>
     <row r="2" spans="1:31" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -13123,7 +13123,7 @@
       <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="93"/>
       <c r="D2" s="12" t="s">
         <v>51</v>
       </c>
@@ -14855,25 +14855,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="74" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -14882,7 +14882,7 @@
       <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="93"/>
       <c r="D2" s="12" t="s">
         <v>51</v>
       </c>
@@ -15161,13 +15161,13 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="71">
+      <c r="B9" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="95">
         <v>0</v>
       </c>
       <c r="D9" s="3">
@@ -15202,9 +15202,9 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="71"/>
+      <c r="A10" s="98"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="95"/>
       <c r="D10" s="3">
         <v>2</v>
       </c>
@@ -15237,9 +15237,9 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="71"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="95"/>
       <c r="D11" s="3">
         <v>3</v>
       </c>
@@ -15641,13 +15641,13 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="78" t="s">
+      <c r="B21" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="71">
+      <c r="C21" s="95">
         <v>0</v>
       </c>
       <c r="D21" s="3">
@@ -15682,9 +15682,9 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="78"/>
-      <c r="B22" s="78"/>
-      <c r="C22" s="71"/>
+      <c r="A22" s="98"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="95"/>
       <c r="D22" s="3">
         <v>2</v>
       </c>
@@ -15717,9 +15717,9 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="78"/>
-      <c r="B23" s="78"/>
-      <c r="C23" s="71"/>
+      <c r="A23" s="98"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="95"/>
       <c r="D23" s="3">
         <v>3</v>
       </c>

</xml_diff>